<commit_message>
fixed the date_published formatting column
</commit_message>
<xml_diff>
--- a/byte_prompt_test_kit/input_output/articles_input.xlsx
+++ b/byte_prompt_test_kit/input_output/articles_input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\Evident-Work\lucas_prompt_testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\Evident-Work\byte_prompt_test_kit\input_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{5BBA4C40-0AC4-4189-8587-B8E6E40BF9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74211157-B345-43C9-A1AB-FB1B7CA53FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,18 +17,14 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'QA relevant articles dataset'!$A$1:$AC$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'QA relevant articles dataset'!$A$1:$AB$13</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="185">
-  <si>
-    <t>temp_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="161">
   <si>
     <t>article_id</t>
   </si>
@@ -81,9 +77,6 @@
     <t>dateTime_found_by_newsapi</t>
   </si>
   <si>
-    <t>dateTimePub</t>
-  </si>
-  <si>
     <t>ingestion_run_datetime</t>
   </si>
   <si>
@@ -112,9 +105,6 @@
   </si>
   <si>
     <t>pillar</t>
-  </si>
-  <si>
-    <t>fd25a19b2e</t>
   </si>
   <si>
     <t>e460462d-fb0a-42a0-8a75-56e63180d2be</t>
@@ -236,9 +226,6 @@
   </si>
   <si>
     <t>Talent</t>
-  </si>
-  <si>
-    <t>f10feeb6e1</t>
   </si>
   <si>
     <t>ab7a20ac-f985-45d1-b2fd-ab0964211974</t>
@@ -289,9 +276,6 @@
     <t>2025-07-29T09:53:19Z</t>
   </si>
   <si>
-    <t>2025-07-29T09:45:58Z</t>
-  </si>
-  <si>
     <t>2025-07-29T15:01:51.813734+00:00</t>
   </si>
   <si>
@@ -333,9 +317,6 @@
     <t>Global Finance magazine\'s free online edition: Country Economic Reports; GDP and trade statistics; Best Banks and Safest Banks; global financial news</t>
   </si>
   <si>
-    <t>728a94c442</t>
-  </si>
-  <si>
     <t>5b8cd374-d919-4c9a-818f-8c500ee8196f</t>
   </si>
   <si>
@@ -378,9 +359,6 @@
     <t>2025-07-30T11:55:51Z</t>
   </si>
   <si>
-    <t>2025-07-30T11:52:12Z</t>
-  </si>
-  <si>
     <t>2025-08-06T11:00:32.778754+00:00</t>
   </si>
   <si>
@@ -402,9 +380,6 @@
   </si>
   <si>
     <t>In-depth analysis, perspective and commentary on key issues affecting the banking industry. (American Banker is an Arizent brand.)</t>
-  </si>
-  <si>
-    <t>6dfb53f0c6</t>
   </si>
   <si>
     <t>60d8c0c2-c3f9-4e25-bcd6-b3c62b5cd120</t>
@@ -486,9 +461,6 @@
     <t>2025-07-10T19:11:27Z</t>
   </si>
   <si>
-    <t>2025-07-10T19:02:29Z</t>
-  </si>
-  <si>
     <t>2025-08-06T11:05:37.967199+00:00</t>
   </si>
   <si>
@@ -558,9 +530,6 @@
     <t>Leadership</t>
   </si>
   <si>
-    <t>d2c15632aa</t>
-  </si>
-  <si>
     <t>a6da4ac8-c5a5-4edc-9772-96c7e5bc1b65</t>
   </si>
   <si>
@@ -614,9 +583,6 @@
     <t>2025-07-29T06:01:28Z</t>
   </si>
   <si>
-    <t>2025-07-29T05:58:31Z</t>
-  </si>
-  <si>
     <t>2025-07-29T15:01:51.048704+00:00</t>
   </si>
   <si>
@@ -642,9 +608,6 @@
  "Hopefully, this time next year, a lot of these engineering problems will be spotted, identified and potentially solved by these agents themselves," he added.</t>
   </si>
   <si>
-    <t>ba037a2120</t>
-  </si>
-  <si>
     <t>c321ed64-7126-44c4-9afe-1a2db283a96f</t>
   </si>
   <si>
@@ -708,9 +671,6 @@
     <t>2025-07-15T13:19:17Z</t>
   </si>
   <si>
-    <t>2025-07-15T13:18:51Z</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Citi's M&amp;A bankers are thriving, DCM bankers are flailing, developers are being displaced It's US banks' results week, and first up today are JPMorgan and Citi. The two banks are disparate beasts.
  Get Morning Coffee ☕ in your inbox. Sign up here.
@@ -739,9 +699,6 @@
     </r>
   </si>
   <si>
-    <t>375959464d</t>
-  </si>
-  <si>
     <t>95ad3879-9f1c-4146-8d30-c9c167b106e7</t>
   </si>
   <si>
@@ -790,9 +747,6 @@
     <t>2025-07-28T21:03:35Z</t>
   </si>
   <si>
-    <t>2025-07-28T20:51:20Z</t>
-  </si>
-  <si>
     <t>2025-07-29T15:01:53.186112+00:00</t>
   </si>
   <si>
@@ -811,9 +765,6 @@
   </si>
   <si>
     <t>New Jersey</t>
-  </si>
-  <si>
-    <t>44c4b729ae</t>
   </si>
   <si>
     <t>74653834-248a-4a9f-abe9-60ac872135da</t>
@@ -859,9 +810,6 @@
     <t>2025-07-11T09:31:59Z</t>
   </si>
   <si>
-    <t>2025-07-11T09:30:01Z</t>
-  </si>
-  <si>
     <t>2025-08-06T11:13:47.969515+00:00</t>
   </si>
   <si>
@@ -887,9 +835,6 @@
   </si>
   <si>
     <t>London</t>
-  </si>
-  <si>
-    <t>a4bfba6cbe</t>
   </si>
   <si>
     <t>5a1235d9-8199-45d3-87ff-a62e455b2896</t>
@@ -948,9 +893,6 @@
     <t>2025-07-21T06:15:25Z</t>
   </si>
   <si>
-    <t>2025-07-21T06:14:12Z</t>
-  </si>
-  <si>
     <t>Interview: Inside HSBC's major 18-month mobile banking app redesign For financial institutions, maintaining digital channels that meet the evolving expectations of customers has become not merely advantageous, but imperative for survival in today's competitive landscape.
  HSBC UK recently undertook a major redesign of its mobile banking app for UK customers with the aim to enhance its digital experience and add new features as it looks to keep pace with the rapid rate of technological advancement and ever-changing customer needs.
  FinTech Futures spoke with George Charalambous, head of digital channels at HSBC UK, to discuss how the bank carried out this redesign and the steps taken to successfully migrate its seven million personal banking customers to the new platform.
@@ -982,9 +924,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>c00f23ed36</t>
-  </si>
-  <si>
     <t>c6e7150b-4f05-4717-b179-ac6d6ad31b07</t>
   </si>
   <si>
@@ -1025,21 +964,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>fintechmagazine.com</t>
-    </r>
-  </si>
-  <si>
     <t>2025-07-10T15:02:19Z</t>
-  </si>
-  <si>
-    <t>2025-07-10T14:33:58Z</t>
   </si>
   <si>
     <t>2025-08-06T11:04:11.683616+00:00</t>
@@ -1055,9 +980,6 @@
  The partnership reflects growing demand for AI solutions that can operate within traditional banking environments. Financial services companies have been cautious about deploying AI technologies due to operational requirements and the need for consistent, accurate outputs.
  UnlikelyAI's approach targets these specific challenges by focusing on reliability and compliance from the outset. The company's technology aims to enable banks to deploy conversational AI while meeting the operational standards that govern financial services.
  The collaboration with Lloyds Banking Group represents a test case for whether neurosymbolic AI can address the fundamental challenges that have limited AI adoption in customer-facing banking applications. The results of the testing phase will inform future deployment decisions.</t>
-  </si>
-  <si>
-    <t>0d4adb9d04</t>
   </si>
   <si>
     <t>102e7745-6320-4740-bb33-75201286f562</t>
@@ -1119,9 +1041,6 @@
     <t>2025-07-27T17:27:11Z</t>
   </si>
   <si>
-    <t>2025-07-27T17:17:31Z</t>
-  </si>
-  <si>
     <t>At JPMorganChase, AI Innovation Is An Operating Committee Mandate Forbes contributors publish independent expert analyses and insights.
  What distinguishes artificial intelligence (AI) leaders from AI followers? A recent survey reported that 89% of Fortune 1000 companies recognize that artificial intelligence (AI) will be the most transformational technology in a generation. Love it or hate it, AI is inevitable. Organizations will need to adapt or risk falling behind.
  JPMorganChase (JPMorgan), the largest U.S. bank with origins tracing back over 225 years to 1799, is seizing upon the moment with a forward-looking long-term vision for AI, which is articulated in the company's mission for the future and embodied at all levels of the organization. This commitment to embracing AI is evident in the composition of the firm's 14-member Operating Committee, where Teresa Heitsenrether occupies a prominent position as chief data and analytics officer (CDAO) for the firm. JPMorgan is at the forefront--very few Fortune 1000 organizations have elevated the CDAO to an operating committee role.
@@ -1153,9 +1072,6 @@
     <t>Reuters</t>
   </si>
   <si>
-    <t>9fc6508647</t>
-  </si>
-  <si>
     <t>5536d676-f98c-43b3-85ac-eedcdf88db21</t>
   </si>
   <si>
@@ -1216,9 +1132,6 @@
     <t>2025-07-29T03:28:41Z</t>
   </si>
   <si>
-    <t>2025-07-29T02:48:36Z</t>
-  </si>
-  <si>
     <t>2025-07-29T15:01:40.529040+00:00</t>
   </si>
   <si>
@@ -1231,6 +1144,12 @@
  ($1 = 1.5328 Australian dollars)
  Reporting by Shivangi Lahiri in Bengaluru; Editing by Sherry Jacob-Phillips
  Our Standards: The Thomson Reuters Trust Principles., opens new tab</t>
+  </si>
+  <si>
+    <t>date_published</t>
+  </si>
+  <si>
+    <t>Fintech Magazine</t>
   </si>
 </sst>
 </file>
@@ -1315,13 +1234,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD4D4D4"/>
-        <bgColor rgb="FFD4D4D4"/>
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
@@ -1353,15 +1272,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1382,7 +1298,16 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1391,6 +1316,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1603,23 +1533,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="6" width="12.59765625" hidden="1"/>
-    <col min="9" max="9" width="58" customWidth="1"/>
-    <col min="10" max="11" width="12.59765625" hidden="1"/>
-    <col min="13" max="18" width="12.59765625" hidden="1"/>
-    <col min="20" max="28" width="12.59765625" hidden="1"/>
+    <col min="1" max="5" width="12.59765625" hidden="1"/>
+    <col min="8" max="8" width="58" customWidth="1"/>
+    <col min="9" max="10" width="12.59765625" hidden="1"/>
+    <col min="12" max="17" width="12.59765625" hidden="1"/>
+    <col min="19" max="27" width="12.59765625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="18.75">
+    <row r="1" spans="1:28" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1672,1119 +1602,1080 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:28" ht="12.75">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="B2" s="3">
+        <v>1025</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="P2" s="7">
+        <v>45865</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" s="3">
+        <v>1</v>
+      </c>
+      <c r="V2" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" ht="13.15">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:28" ht="12.75">
+      <c r="A3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1011</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="4">
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="P3" s="7">
+        <v>45867</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="9">
+        <v>45867</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" s="3">
+        <v>1</v>
+      </c>
+      <c r="V3" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="12.75">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1050</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="3">
+        <v>385090</v>
+      </c>
+      <c r="P4" s="7">
+        <v>45868</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="9">
+        <v>45868</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="T4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U4" s="3">
+        <v>1</v>
+      </c>
+      <c r="V4" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB4" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="12.75">
+      <c r="A5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1019</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="3">
+        <v>333755</v>
+      </c>
+      <c r="P5" s="7">
+        <v>45848</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R5" s="9">
+        <v>45848</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="T5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U5" s="3">
+        <v>1</v>
+      </c>
+      <c r="V5" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB5" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="12.75">
+      <c r="A6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="3">
         <v>1025</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O6" s="3">
+        <v>213198</v>
+      </c>
+      <c r="P6" s="7">
+        <v>45867</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R6" s="9">
+        <v>45867</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="T6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" s="3">
+        <v>1</v>
+      </c>
+      <c r="V6" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB6" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="12.75">
+      <c r="A7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1004</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="4">
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="3">
         <v>1000000</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="P7" s="7">
+        <v>45853</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="R7" s="9">
+        <v>45853</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="T7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
+        <v>1</v>
+      </c>
+      <c r="V7" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB7" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="12.75">
+      <c r="A8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1019</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="O8" s="3">
+        <v>90000</v>
+      </c>
+      <c r="P8" s="7">
+        <v>45866</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="R8" s="9">
+        <v>45866</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="T8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U8" s="3">
+        <v>1</v>
+      </c>
+      <c r="V8" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB8" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="12.75">
+      <c r="A9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1022</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="O9" s="3">
+        <v>14205</v>
+      </c>
+      <c r="P9" s="7">
+        <v>45849</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="R9" s="9">
+        <v>45849</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="T9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" s="3">
+        <v>1</v>
+      </c>
+      <c r="V9" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W9" s="3">
+        <v>0</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB9" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="12.75">
+      <c r="A10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1024</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="O10" s="3">
+        <v>376957</v>
+      </c>
+      <c r="P10" s="7">
+        <v>45859</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="R10" s="9">
+        <v>45859</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="T10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U10" s="3">
+        <v>1</v>
+      </c>
+      <c r="V10" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W10" s="3">
+        <v>0</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB10" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="12.75">
+      <c r="A11" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1052</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O11" s="3">
+        <v>392624</v>
+      </c>
+      <c r="P11" s="7">
+        <v>45848</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="R11" s="9">
+        <v>45848</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="T11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U11" s="3">
+        <v>1</v>
+      </c>
+      <c r="V11" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W11" s="3">
+        <v>0</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB11" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="12.75">
+      <c r="A12" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1004</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O12" s="3">
+        <v>13995</v>
+      </c>
+      <c r="P12" s="7">
         <v>45865</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="Q12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="R12" s="9">
+        <v>45865</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="T12" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" s="3">
+        <v>1</v>
+      </c>
+      <c r="V12" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W12" s="3">
+        <v>0</v>
+      </c>
+      <c r="X12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="Y12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB12" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="12.75">
+      <c r="A13" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1064</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="O13" s="3">
+        <v>4500</v>
+      </c>
+      <c r="P13" s="7">
+        <v>45867</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="R13" s="9">
+        <v>45867</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="T13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U13" s="3">
+        <v>1</v>
+      </c>
+      <c r="V13" s="8">
+        <v>45875.590978557142</v>
+      </c>
+      <c r="W13" s="3">
+        <v>0</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB13" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="U2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V2" s="4">
-        <v>1</v>
-      </c>
-      <c r="W2" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="13.15">
-      <c r="A3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1011</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>45867</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V3" s="4">
-        <v>1</v>
-      </c>
-      <c r="W3" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC3" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="13.15">
-      <c r="A4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1050</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="P4" s="4">
-        <v>385090</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>45868</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="U4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V4" s="4">
-        <v>1</v>
-      </c>
-      <c r="W4" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC4" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" ht="13.15">
-      <c r="A5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1019</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="P5" s="4">
-        <v>333755</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>45848</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="U5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V5" s="4">
-        <v>1</v>
-      </c>
-      <c r="W5" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC5" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" ht="13.15">
-      <c r="A6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1025</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="P6" s="4">
-        <v>213198</v>
-      </c>
-      <c r="Q6" s="8">
-        <v>45867</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="U6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V6" s="4">
-        <v>1</v>
-      </c>
-      <c r="W6" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X6" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC6" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" ht="13.15">
-      <c r="A7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1004</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>45853</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="U7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V7" s="4">
-        <v>1</v>
-      </c>
-      <c r="W7" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X7" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC7" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" ht="13.15">
-      <c r="A8" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1019</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="P8" s="4">
-        <v>90000</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>45866</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V8" s="4">
-        <v>1</v>
-      </c>
-      <c r="W8" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z8" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AC8" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" ht="13.15">
-      <c r="A9" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1022</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P9" s="4">
-        <v>14205</v>
-      </c>
-      <c r="Q9" s="8">
-        <v>45849</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="S9" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="U9" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V9" s="4">
-        <v>1</v>
-      </c>
-      <c r="W9" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X9" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z9" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="AC9" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" ht="13.15">
-      <c r="A10" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1024</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="P10" s="4">
-        <v>376957</v>
-      </c>
-      <c r="Q10" s="8">
-        <v>45859</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="S10" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="U10" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V10" s="4">
-        <v>1</v>
-      </c>
-      <c r="W10" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z10" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="AC10" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="13.15">
-      <c r="A11" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1052</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="N11" s="7"/>
-      <c r="O11" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="P11" s="4">
-        <v>392624</v>
-      </c>
-      <c r="Q11" s="8">
-        <v>45848</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="U11" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V11" s="4">
-        <v>1</v>
-      </c>
-      <c r="W11" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X11" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z11" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AC11" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="13.15">
-      <c r="A12" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1004</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P12" s="4">
-        <v>13995</v>
-      </c>
-      <c r="Q12" s="8">
-        <v>45865</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="S12" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="U12" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V12" s="4">
-        <v>1</v>
-      </c>
-      <c r="W12" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X12" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z12" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="AC12" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" ht="13.15">
-      <c r="A13" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1064</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="P13" s="4">
-        <v>4500</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>45867</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="S13" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="U13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V13" s="4">
-        <v>1</v>
-      </c>
-      <c r="W13" s="9">
-        <v>45875.590978557142</v>
-      </c>
-      <c r="X13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z13" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="AC13" s="10" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC13" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:AB13" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="J2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="AB2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="J3" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="G4" r:id="rId7" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="J4" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="G5" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="J5" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="G6" r:id="rId11" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="J6" r:id="rId12" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="G7" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="I7" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="J7" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="AB7" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G8" r:id="rId17" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="J8" r:id="rId18" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G9" r:id="rId19" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="J9" r:id="rId20" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="G10" r:id="rId21" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="J10" r:id="rId22" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="G11" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="J11" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="L11" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="G12" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="J12" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="G13" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
-    <hyperlink ref="J13" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
-    <hyperlink ref="M13" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="I2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="AA2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="I3" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="F4" r:id="rId7" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="I4" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="F5" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="I5" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="F6" r:id="rId11" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="I6" r:id="rId12" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="F7" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="H7" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="I7" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="AA7" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="F8" r:id="rId17" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="I8" r:id="rId18" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="I9" r:id="rId20" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="F10" r:id="rId21" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="I10" r:id="rId22" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="F11" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="I11" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="K11" r:id="rId25" display="fintechmagazine.com" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="F12" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="I12" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="F13" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="I13" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="L13" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2803,6 +2694,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d8004025-247d-462d-917e-4507883b73d1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007E2F816B15CE57488A1CD3FB168E8F73" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7caab64fe9e9af70387a8a9553b6f8d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d8004025-247d-462d-917e-4507883b73d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6492697f6841657b31da2ed0e192b85c" ns3:_="">
     <xsd:import namespace="d8004025-247d-462d-917e-4507883b73d1"/>
@@ -2958,24 +2866,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADE2B69-BD5A-4062-9B5A-4FA92CCEA4BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d8004025-247d-462d-917e-4507883b73d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d8004025-247d-462d-917e-4507883b73d1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0697DFC8-4458-4268-88DC-EFCC48FA7497}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F70B96F5-3857-4C90-A61B-BB8CAE68AD1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2991,28 +2906,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0697DFC8-4458-4268-88DC-EFCC48FA7497}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ADE2B69-BD5A-4062-9B5A-4FA92CCEA4BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d8004025-247d-462d-917e-4507883b73d1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>